<commit_message>
feat: use sheetjs.ssf to parse number format
</commit_message>
<xml_diff>
--- a/tests/features/data/cell/formatted.xlsx
+++ b/tests/features/data/cell/formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TiPlus7100/Devs/rexllent/tests/data/cell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE5172C-A162-E04C-B257-42C199395688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D38A929-E3EC-674D-9C71-30737AD52AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22220" yWindow="10840" windowWidth="11660" windowHeight="8680" xr2:uid="{16C3D092-66B8-1744-A9D0-696A0D662A80}"/>
+    <workbookView xWindow="13920" yWindow="2560" windowWidth="11660" windowHeight="8680" xr2:uid="{16C3D092-66B8-1744-A9D0-696A0D662A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,36 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -79,7 +105,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -93,6 +119,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -429,21 +458,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2643C81-D7B0-2E4F-8D79-B94379B7C6AE}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2">
         <v>123</v>
       </c>
@@ -451,27 +480,33 @@
         <v>2.21313</v>
       </c>
       <c r="C1" s="4">
-        <v>0.43078703703703702</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <v>3.3999999999999998E-3</v>
       </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>34</v>
       </c>
       <c r="B2" s="3">
         <v>2424</v>
       </c>
-      <c r="C2" s="4">
-        <v>45638</v>
+      <c r="C2" s="5">
+        <v>45639</v>
       </c>
       <c r="D2" s="1">
         <v>0.68</v>
       </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>234</v>
       </c>
@@ -484,8 +519,11 @@
       <c r="D3" s="1">
         <v>29.29</v>
       </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -495,9 +533,15 @@
       <c r="D4" s="1">
         <v>0.28999999999999998</v>
       </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add number formatting support and update XLSX parsing
- Introduced a new `numfmt.typ` file to handle number formatting using JavaScript functions.
- Renamed the `render` function to `format` in `ssf.typ` for consistency with the new number formatting.
- Updated the `formatted.xlsx` file to reflect changes in formatting.
- Modified test cases in `test.typ` to use the new `parse-formatted-cell` option for XLSX parsing, ensuring compatibility with the updated formatting logic.
</commit_message>
<xml_diff>
--- a/tests/features/data/cell/formatted.xlsx
+++ b/tests/features/data/cell/formatted.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TiPlus7100/Devs/rexllent/tests/data/cell/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TiPlus7100/Devs/rexllent/tests/features/data/cell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D38A929-E3EC-674D-9C71-30737AD52AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2103CD8-1802-7E41-8891-0FA0525761D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="2560" windowWidth="11660" windowHeight="8680" xr2:uid="{16C3D092-66B8-1744-A9D0-696A0D662A80}"/>
+    <workbookView xWindow="24780" yWindow="8860" windowWidth="11660" windowHeight="8680" xr2:uid="{16C3D092-66B8-1744-A9D0-696A0D662A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,14 +57,23 @@
     <t>e</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>foo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="7">
+    <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;¥&quot;* #,##0.00_);_(&quot;¥&quot;* \(#,##0.00\);_(&quot;¥&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="181" formatCode="_ [$₹-44F]\ * #,##0.00_ ;_ [$₹-44F]\ * \-#,##0.00_ ;_ [$₹-44F]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="\$#,##0.00;[Red]\$#,##0.00"/>
+    <numFmt numFmtId="184" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -105,7 +114,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -121,7 +130,28 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2643C81-D7B0-2E4F-8D79-B94379B7C6AE}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -470,9 +500,10 @@
     <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2">
         <v>123</v>
       </c>
@@ -488,9 +519,12 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2">
+    <row r="2" spans="1:6">
+      <c r="A2" s="9">
         <v>34</v>
       </c>
       <c r="B2" s="3">
@@ -505,9 +539,12 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2">
+    <row r="3" spans="1:6">
+      <c r="A3" s="10">
         <v>234</v>
       </c>
       <c r="B3" s="3">
@@ -522,9 +559,12 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
+    <row r="4" spans="1:6">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="3">
@@ -536,10 +576,13 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2">
-        <v>4</v>
+    <row r="5" spans="1:6">
+      <c r="A5" s="12">
+        <v>-4</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Remove unused SSF type definition and update tests
- Deleted the ssf.typ file as it was no longer needed.
- Updated the formatted.xlsx file to reflect changes in cell formatting.
- Updated the reference image 7.png to match the latest output.
- Removed the locale parameter from the xlsx-parser call in test.typ to simplify the test case.
</commit_message>
<xml_diff>
--- a/tests/features/data/cell/formatted.xlsx
+++ b/tests/features/data/cell/formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TiPlus7100/Devs/rexllent/tests/features/data/cell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2103CD8-1802-7E41-8891-0FA0525761D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F444463E-C354-8F4D-83BE-2068132CB8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24780" yWindow="8860" windowWidth="11660" windowHeight="8680" xr2:uid="{16C3D092-66B8-1744-A9D0-696A0D662A80}"/>
+    <workbookView xWindow="6200" yWindow="6940" windowWidth="11660" windowHeight="8680" xr2:uid="{16C3D092-66B8-1744-A9D0-696A0D662A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,14 +66,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;¥&quot;* #,##0.00_);_(&quot;¥&quot;* \(#,##0.00\);_(&quot;¥&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="181" formatCode="_ [$₹-44F]\ * #,##0.00_ ;_ [$₹-44F]\ * \-#,##0.00_ ;_ [$₹-44F]\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="\$#,##0.00;[Red]\$#,##0.00"/>
-    <numFmt numFmtId="184" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="_ [$₹-44F]\ * #,##0.00_ ;_ [$₹-44F]\ * \-#,##0.00_ ;_ [$₹-44F]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="\$#,##0.00;[Red]\$#,##0.00"/>
+    <numFmt numFmtId="180" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
+    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="186" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="187" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -114,7 +116,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -130,9 +132,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -145,13 +144,22 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -491,16 +499,16 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="10.83203125" style="6"/>
+    <col min="6" max="6" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -510,7 +518,7 @@
       <c r="B1" s="3">
         <v>2.21313</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="13">
         <v>1</v>
       </c>
       <c r="D1" s="1">
@@ -519,18 +527,18 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>34</v>
       </c>
       <c r="B2" s="3">
         <v>2424</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="12">
         <v>45639</v>
       </c>
       <c r="D2" s="1">
@@ -539,18 +547,18 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>234</v>
       </c>
       <c r="B3" s="3">
         <v>214</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="14">
         <v>45758</v>
       </c>
       <c r="D3" s="1">
@@ -559,12 +567,12 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="3">
@@ -576,12 +584,12 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>-4</v>
       </c>
       <c r="E5" t="s">

</xml_diff>